<commit_message>
Facture Excel (avant test)
</commit_message>
<xml_diff>
--- a/App_pressing_Loreau/Resources/PatternExcel/FacturePattern.xlsx
+++ b/App_pressing_Loreau/Resources/PatternExcel/FacturePattern.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700"/>
@@ -11,15 +11,71 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="12">
+  <si>
+    <t>LE LOREAU 28130 Hanches</t>
+  </si>
+  <si>
+    <t>BLEU Pressing</t>
+  </si>
+  <si>
+    <t>Siret : 49535155300021</t>
+  </si>
+  <si>
+    <t>Facture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ref : </t>
+  </si>
+  <si>
+    <t>&lt;Reference&gt;</t>
+  </si>
+  <si>
+    <t>Adresse 1</t>
+  </si>
+  <si>
+    <t>Adresse 3</t>
+  </si>
+  <si>
+    <t>Adresse 2</t>
+  </si>
+  <si>
+    <t>&lt;Nom Type Article&gt;</t>
+  </si>
+  <si>
+    <t>&lt;TTC&gt;</t>
+  </si>
+  <si>
+    <t>Nom Prenom</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -34,7 +90,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -42,12 +98,187 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="double">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="double">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="double">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -60,7 +291,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Bureau">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -98,7 +329,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Bureau">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -168,7 +399,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Bureau">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -342,14 +573,358 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A2:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="10" width="7.42578125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" ht="18.75">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" ht="26.25">
+      <c r="A6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickTop="1">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickTop="1">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+      <c r="G18" s="16"/>
+      <c r="I18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="G19" s="16"/>
+      <c r="I19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
+      <c r="G20" s="16"/>
+      <c r="I20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
+      <c r="G21" s="16"/>
+      <c r="I21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="7"/>
+      <c r="G22" s="16"/>
+      <c r="I22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="7"/>
+      <c r="G23" s="16"/>
+      <c r="I23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="7"/>
+      <c r="G24" s="16"/>
+      <c r="I24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="7"/>
+      <c r="G25" s="16"/>
+      <c r="I25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="7"/>
+      <c r="G26" s="16"/>
+      <c r="I26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="7"/>
+      <c r="G27" s="16"/>
+      <c r="I27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="7"/>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="7"/>
+      <c r="G28" s="16"/>
+      <c r="I28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="7"/>
+      <c r="G29" s="16"/>
+      <c r="I29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="7"/>
+      <c r="G30" s="16"/>
+      <c r="I30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="7"/>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="7"/>
+      <c r="G31" s="16"/>
+      <c r="I31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J31" s="7"/>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="7"/>
+      <c r="G32" s="16"/>
+      <c r="I32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J32" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="37">
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A11:D11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>